<commit_message>
agregar CSVs y modificar Python
</commit_message>
<xml_diff>
--- a/datos/numeros.xlsx
+++ b/datos/numeros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f7ba5ab37b782061/Estudios/UNI/Curso NLP/Proyecto/Traductor-Quechua-Spanish-Spanish-Quechua/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{EB4F5C7A-4E50-41F3-A114-B425A718F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C56B5C27-72ED-4433-93C9-DDD86942A295}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{EB4F5C7A-4E50-41F3-A114-B425A718F4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1FAA20E-17F7-4854-89BF-7DF147511BB9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{89CFB379-E681-4DDB-A372-18C4CA2DE17D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t>cero</t>
   </si>
@@ -249,6 +249,36 @@
   </si>
   <si>
     <t>tawa pachak</t>
+  </si>
+  <si>
+    <t>sesenta</t>
+  </si>
+  <si>
+    <t>setenta</t>
+  </si>
+  <si>
+    <t>ochenta</t>
+  </si>
+  <si>
+    <t>quinientos</t>
+  </si>
+  <si>
+    <t>mil</t>
+  </si>
+  <si>
+    <t>un millón</t>
+  </si>
+  <si>
+    <t>suqta chunka</t>
+  </si>
+  <si>
+    <t>qanchis chunka</t>
+  </si>
+  <si>
+    <t>pusaq chunka</t>
+  </si>
+  <si>
+    <t>pusaq</t>
   </si>
 </sst>
 </file>
@@ -284,9 +314,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,6 +331,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,303 +634,339 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E8A327-F342-46AD-83C9-7E4747FF6910}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>28</v>
+      <c r="B9" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" t="s">
         <v>44</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="A27" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>49</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B33" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B35" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>52</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B36" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>53</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B37" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>54</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B39" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>